<commit_message>
Bai 23 - Excel file - DataProvider
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data/data.xlsx
+++ b/src/test/resources/test_data/data.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\Appium\AppiumJava122024_Multi_Platform\src\test\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6B3016-563A-4EDE-B48A-CC0F548F9C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4837142-1BC4-4483-A50B-C9C65ABF8010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{5D795E49-F5D6-486B-B630-D84533204838}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{5D795E49-F5D6-486B-B630-D84533204838}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>PASSWORD</t>
   </si>
@@ -78,27 +78,17 @@
   </si>
   <si>
     <t>123456</t>
-  </si>
-  <si>
-    <t>EXPECTED_RESULT</t>
-  </si>
-  <si>
-    <t>Passed</t>
-  </si>
-  <si>
-    <t>Failed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -107,20 +97,17 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill/>
     </fill>
   </fills>
   <borders count="1">
@@ -135,28 +122,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -175,9 +144,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -215,7 +184,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -321,7 +290,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -463,7 +432,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -471,53 +440,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D00ADF3-05D6-490F-B407-73CD8AAE07B7}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.35546875"/>
-    <col min="2" max="2" customWidth="true" width="15.5703125"/>
+    <col min="1" max="1" width="14.3828125" customWidth="1"/>
+    <col min="2" max="2" width="15.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s" s="4">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s" s="0">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s" s="0">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s" s="0">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -537,13 +497,13 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.2109375"/>
-    <col min="2" max="2" customWidth="true" width="11.5703125"/>
+    <col min="1" max="1" width="15.23046875" customWidth="1"/>
+    <col min="2" max="2" width="11.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -551,16 +511,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -581,13 +541,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.0703125"/>
-    <col min="2" max="2" customWidth="true" width="13.42578125"/>
+    <col min="1" max="1" width="15.07421875" customWidth="1"/>
+    <col min="2" max="2" width="13.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -595,16 +555,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">

</xml_diff>

<commit_message>
Bài 23 - Excel File + DataProvider Full
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data/data.xlsx
+++ b/src/test/resources/test_data/data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\Appium\AppiumJava122024_Multi_Platform\src\test\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4837142-1BC4-4483-A50B-C9C65ABF8010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEDA7BB-7577-455C-BBA2-EEA04634D390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{5D795E49-F5D6-486B-B630-D84533204838}"/>
+    <workbookView xWindow="4452" yWindow="2304" windowWidth="22704" windowHeight="13872" activeTab="3" xr2:uid="{5D795E49-F5D6-486B-B630-D84533204838}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Table" sheetId="2" r:id="rId2"/>
     <sheet name="Product" sheetId="3" r:id="rId3"/>
+    <sheet name="Login_Excel" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>PASSWORD</t>
   </si>
@@ -78,6 +79,36 @@
   </si>
   <si>
     <t>123456</t>
+  </si>
+  <si>
+    <t>EXPECTED_RESULT</t>
+  </si>
+  <si>
+    <t>TEST_CASE</t>
+  </si>
+  <si>
+    <t>testLoginSuccess</t>
+  </si>
+  <si>
+    <t>testLoginFailWithUsernameInvalid</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>password1</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>password2</t>
+  </si>
+  <si>
+    <t>admin456</t>
   </si>
 </sst>
 </file>
@@ -102,12 +133,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
     </fill>
   </fills>
   <borders count="1">
@@ -122,10 +156,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,10 +477,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D00ADF3-05D6-490F-B407-73CD8AAE07B7}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.765625" customWidth="1"/>
+    <col min="2" max="2" width="14.3828125" customWidth="1"/>
+    <col min="3" max="3" width="15.53515625" customWidth="1"/>
+    <col min="4" max="4" width="18.61328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.3046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B107806-66B4-428E-AC5D-CABDBFEA3B5F}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.23046875" customWidth="1"/>
+    <col min="2" max="2" width="11.53515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{323FF40E-AC40-4CE0-976A-4D81751C5FB9}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.3828125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D73DB64-A9D1-467E-9003-CD4C952118F0}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -478,97 +674,26 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B107806-66B4-428E-AC5D-CABDBFEA3B5F}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.23046875" customWidth="1"/>
-    <col min="2" max="2" width="11.53515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{323FF40E-AC40-4CE0-976A-4D81751C5FB9}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.07421875" customWidth="1"/>
-    <col min="2" max="2" width="13.3828125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>